<commit_message>
Added version 3.2.0 publication
</commit_message>
<xml_diff>
--- a/fhir/core/CodeSystem-DkCoreProfessionGroupCodes.xlsx
+++ b/fhir/core/CodeSystem-DkCoreProfessionGroupCodes.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>3.1.0</t>
+    <t>3.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-08T21:51:35+01:00</t>
+    <t>2024-05-06T15:28:33+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,7 +72,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>HL7 Denmark (http://www.hl7.dk, jenskristianvilladsen@gmail.com)</t>
   </si>
   <si>
     <t>Jurisdiction</t>

</xml_diff>